<commit_message>
improved setup and data_cleaning modules
1_setup.R now includes a config file driven option to load a custom vulnerability and outcome generating script which should be called directly in the 2_data_cleaning.R module.  Improved error handling for importing raw survey files.  Updated template for the config - template.yml file.  Misc helper scripts added to the adhoc_scripts folder
</commit_message>
<xml_diff>
--- a/analyses/a_new_analysis_template/pathways data dictionary.xlsx
+++ b/analyses/a_new_analysis_template/pathways data dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/Documents/GitHub/pathways-segmentation/analyses/a-new-analysis-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/Documents/GitHub/pathways-segmentation-public/analyses/a_new_analysis_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2700" documentId="8_{D23518CC-E1D3-4ECE-9E98-7428ECDD5F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92CCFB35-0D69-4AB0-9D73-F3268D291308}"/>
+  <xr:revisionPtr revIDLastSave="2707" documentId="8_{D23518CC-E1D3-4ECE-9E98-7428ECDD5F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9938B78A-858B-4386-96D6-D11F6993C6BF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">outcomes!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">vulnerabilities!$A$1:$I$501</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">vulnerabilities!$A$1:$I$502</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="1770">
   <si>
     <t>category</t>
   </si>
@@ -5348,6 +5348,9 @@
   </si>
   <si>
     <t>Categorical variable for woman decision making index</t>
+  </si>
+  <si>
+    <t>Location of the household toilet</t>
   </si>
 </sst>
 </file>
@@ -7505,11 +7508,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I501"/>
+  <dimension ref="A1:I502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C500" sqref="C500"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F310" sqref="F310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11845,13 +11848,13 @@
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>1676</v>
+        <v>901</v>
       </c>
       <c r="B309" t="s">
-        <v>1677</v>
+        <v>1625</v>
       </c>
       <c r="C309" t="s">
-        <v>1730</v>
+        <v>1769</v>
       </c>
       <c r="F309">
         <v>1</v>
@@ -11859,24 +11862,27 @@
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>330</v>
+        <v>1676</v>
       </c>
       <c r="B310" t="s">
-        <v>826</v>
+        <v>1677</v>
       </c>
       <c r="C310" t="s">
-        <v>827</v>
-      </c>
-      <c r="G310">
+        <v>1730</v>
+      </c>
+      <c r="F310">
         <v>1</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>828</v>
+        <v>330</v>
       </c>
       <c r="B311" t="s">
-        <v>1550</v>
+        <v>826</v>
+      </c>
+      <c r="C311" t="s">
+        <v>827</v>
       </c>
       <c r="G311">
         <v>1</v>
@@ -11884,13 +11890,10 @@
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>331</v>
+        <v>828</v>
       </c>
       <c r="B312" t="s">
-        <v>1551</v>
-      </c>
-      <c r="C312" t="s">
-        <v>1731</v>
+        <v>1550</v>
       </c>
       <c r="G312">
         <v>1</v>
@@ -11898,13 +11901,13 @@
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B313" t="s">
-        <v>333</v>
+        <v>1551</v>
       </c>
       <c r="C313" t="s">
-        <v>334</v>
+        <v>1731</v>
       </c>
       <c r="G313">
         <v>1</v>
@@ -11912,13 +11915,13 @@
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B314" t="s">
-        <v>1552</v>
+        <v>333</v>
       </c>
       <c r="C314" t="s">
-        <v>1557</v>
+        <v>334</v>
       </c>
       <c r="G314">
         <v>1</v>
@@ -11926,13 +11929,13 @@
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B315" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C315" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="G315">
         <v>1</v>
@@ -11940,13 +11943,13 @@
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B316" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C316" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="G316">
         <v>1</v>
@@ -11954,13 +11957,13 @@
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B317" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C317" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="G317">
         <v>1</v>
@@ -11968,13 +11971,13 @@
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B318" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C318" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="G318">
         <v>1</v>
@@ -11982,41 +11985,41 @@
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B319" t="s">
-        <v>341</v>
+        <v>1556</v>
       </c>
       <c r="C319" t="s">
-        <v>342</v>
-      </c>
-      <c r="F319">
+        <v>1561</v>
+      </c>
+      <c r="G319">
         <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>829</v>
+        <v>340</v>
       </c>
       <c r="B320" t="s">
-        <v>1562</v>
+        <v>341</v>
       </c>
       <c r="C320" t="s">
-        <v>830</v>
-      </c>
-      <c r="G320">
+        <v>342</v>
+      </c>
+      <c r="F320">
         <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>1273</v>
+        <v>829</v>
       </c>
       <c r="B321" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C321" t="s">
-        <v>1274</v>
+        <v>830</v>
       </c>
       <c r="G321">
         <v>1</v>
@@ -12024,13 +12027,13 @@
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>343</v>
+        <v>1273</v>
       </c>
       <c r="B322" t="s">
-        <v>344</v>
+        <v>1563</v>
       </c>
       <c r="C322" t="s">
-        <v>345</v>
+        <v>1274</v>
       </c>
       <c r="G322">
         <v>1</v>
@@ -12038,13 +12041,13 @@
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B323" t="s">
-        <v>831</v>
+        <v>344</v>
       </c>
       <c r="C323" t="s">
-        <v>832</v>
+        <v>345</v>
       </c>
       <c r="G323">
         <v>1</v>
@@ -12052,27 +12055,27 @@
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B324" t="s">
-        <v>348</v>
+        <v>831</v>
       </c>
       <c r="C324" t="s">
-        <v>349</v>
-      </c>
-      <c r="E324">
+        <v>832</v>
+      </c>
+      <c r="G324">
         <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B325" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C325" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E325">
         <v>1</v>
@@ -12080,13 +12083,13 @@
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B326" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C326" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E326">
         <v>1</v>
@@ -12094,13 +12097,13 @@
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B327" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C327" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E327">
         <v>1</v>
@@ -12108,13 +12111,13 @@
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>833</v>
+        <v>356</v>
       </c>
       <c r="B328" t="s">
-        <v>1564</v>
+        <v>357</v>
       </c>
       <c r="C328" t="s">
-        <v>1732</v>
+        <v>358</v>
       </c>
       <c r="E328">
         <v>1</v>
@@ -12122,13 +12125,13 @@
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B329" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C329" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="E329">
         <v>1</v>
@@ -12136,13 +12139,13 @@
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>359</v>
+        <v>834</v>
       </c>
       <c r="B330" t="s">
-        <v>360</v>
+        <v>1565</v>
       </c>
       <c r="C330" t="s">
-        <v>361</v>
+        <v>1733</v>
       </c>
       <c r="E330">
         <v>1</v>
@@ -12150,13 +12153,13 @@
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>1076</v>
+        <v>359</v>
       </c>
       <c r="B331" t="s">
-        <v>1566</v>
+        <v>360</v>
       </c>
       <c r="C331" t="s">
-        <v>1077</v>
+        <v>361</v>
       </c>
       <c r="E331">
         <v>1</v>
@@ -12164,13 +12167,13 @@
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>836</v>
+        <v>1076</v>
       </c>
       <c r="B332" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C332" t="s">
-        <v>1733</v>
+        <v>1077</v>
       </c>
       <c r="E332">
         <v>1</v>
@@ -12178,13 +12181,13 @@
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>1078</v>
+        <v>836</v>
       </c>
       <c r="B333" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C333" t="s">
-        <v>1079</v>
+        <v>1733</v>
       </c>
       <c r="E333">
         <v>1</v>
@@ -12192,13 +12195,13 @@
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>837</v>
+        <v>1078</v>
       </c>
       <c r="B334" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C334" t="s">
-        <v>1733</v>
+        <v>1079</v>
       </c>
       <c r="E334">
         <v>1</v>
@@ -12206,10 +12209,10 @@
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B335" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C335" t="s">
         <v>1733</v>
@@ -12220,10 +12223,10 @@
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B336" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C336" t="s">
         <v>1733</v>
@@ -12234,13 +12237,13 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>362</v>
+        <v>839</v>
       </c>
       <c r="B337" t="s">
-        <v>363</v>
+        <v>1571</v>
       </c>
       <c r="C337" t="s">
-        <v>840</v>
+        <v>1733</v>
       </c>
       <c r="E337">
         <v>1</v>
@@ -12248,13 +12251,13 @@
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>841</v>
+        <v>362</v>
       </c>
       <c r="B338" t="s">
-        <v>842</v>
+        <v>363</v>
       </c>
       <c r="C338" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="E338">
         <v>1</v>
@@ -12262,13 +12265,13 @@
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B339" t="s">
-        <v>1572</v>
+        <v>842</v>
       </c>
       <c r="C339" t="s">
-        <v>1733</v>
+        <v>835</v>
       </c>
       <c r="E339">
         <v>1</v>
@@ -12276,27 +12279,27 @@
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>1275</v>
+        <v>843</v>
       </c>
       <c r="B340" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C340" t="s">
-        <v>1276</v>
-      </c>
-      <c r="H340">
+        <v>1733</v>
+      </c>
+      <c r="E340">
         <v>1</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B341" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C341" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="H341">
         <v>1</v>
@@ -12304,27 +12307,27 @@
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>844</v>
+        <v>1277</v>
       </c>
       <c r="B342" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C342" t="s">
-        <v>1734</v>
-      </c>
-      <c r="G342">
+        <v>1278</v>
+      </c>
+      <c r="H342">
         <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B343" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C343" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="G343">
         <v>1</v>
@@ -12332,63 +12335,66 @@
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>364</v>
+        <v>845</v>
       </c>
       <c r="B344" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C344" t="s">
-        <v>1736</v>
-      </c>
-      <c r="E344">
+        <v>1735</v>
+      </c>
+      <c r="G344">
         <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B345" t="s">
-        <v>366</v>
+        <v>1577</v>
       </c>
       <c r="C345" t="s">
-        <v>846</v>
-      </c>
-      <c r="H345">
+        <v>1736</v>
+      </c>
+      <c r="E345">
         <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>1080</v>
+        <v>365</v>
       </c>
       <c r="B346" t="s">
-        <v>1578</v>
+        <v>366</v>
       </c>
       <c r="C346" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E346">
+        <v>846</v>
+      </c>
+      <c r="H346">
         <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>847</v>
+        <v>1080</v>
       </c>
       <c r="B347" t="s">
-        <v>1579</v>
-      </c>
-      <c r="G347">
+        <v>1578</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E347">
         <v>1</v>
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B348" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="G348">
         <v>1</v>
@@ -12396,41 +12402,38 @@
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>1133</v>
+        <v>848</v>
       </c>
       <c r="B349" t="s">
-        <v>1581</v>
-      </c>
-      <c r="C349" t="s">
-        <v>1134</v>
-      </c>
-      <c r="H349">
+        <v>1580</v>
+      </c>
+      <c r="G349">
         <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>367</v>
+        <v>1133</v>
       </c>
       <c r="B350" t="s">
-        <v>1373</v>
+        <v>1581</v>
       </c>
       <c r="C350" t="s">
-        <v>1374</v>
-      </c>
-      <c r="D350">
+        <v>1134</v>
+      </c>
+      <c r="H350">
         <v>1</v>
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B351" t="s">
-        <v>369</v>
+        <v>1373</v>
       </c>
       <c r="C351" t="s">
-        <v>849</v>
+        <v>1374</v>
       </c>
       <c r="D351">
         <v>1</v>
@@ -12438,13 +12441,13 @@
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B352" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C352" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D352">
         <v>1</v>
@@ -12452,13 +12455,13 @@
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>1179</v>
+        <v>370</v>
       </c>
       <c r="B353" t="s">
-        <v>1582</v>
+        <v>371</v>
       </c>
       <c r="C353" t="s">
-        <v>1180</v>
+        <v>850</v>
       </c>
       <c r="D353">
         <v>1</v>
@@ -12466,41 +12469,41 @@
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>851</v>
+        <v>1179</v>
       </c>
       <c r="B354" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C354" t="s">
-        <v>1737</v>
-      </c>
-      <c r="H354">
+        <v>1180</v>
+      </c>
+      <c r="D354">
         <v>1</v>
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>372</v>
+        <v>851</v>
       </c>
       <c r="B355" t="s">
-        <v>373</v>
+        <v>1583</v>
       </c>
       <c r="C355" t="s">
-        <v>852</v>
-      </c>
-      <c r="E355">
+        <v>1737</v>
+      </c>
+      <c r="H355">
         <v>1</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B356" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C356" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E356">
         <v>1</v>
@@ -12508,13 +12511,13 @@
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B357" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C357" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E357">
         <v>1</v>
@@ -12522,13 +12525,13 @@
     </row>
     <row r="358" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B358" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C358" t="s">
-        <v>380</v>
+        <v>854</v>
       </c>
       <c r="E358">
         <v>1</v>
@@ -12536,13 +12539,13 @@
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B359" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C359" t="s">
-        <v>855</v>
+        <v>380</v>
       </c>
       <c r="E359">
         <v>1</v>
@@ -12550,41 +12553,41 @@
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B360" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C360" t="s">
-        <v>385</v>
-      </c>
-      <c r="F360">
+        <v>855</v>
+      </c>
+      <c r="E360">
         <v>1</v>
       </c>
     </row>
     <row r="361" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>856</v>
+        <v>383</v>
       </c>
       <c r="B361" t="s">
-        <v>1375</v>
+        <v>384</v>
       </c>
       <c r="C361" t="s">
-        <v>1376</v>
-      </c>
-      <c r="G361">
+        <v>385</v>
+      </c>
+      <c r="F361">
         <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>386</v>
+        <v>856</v>
       </c>
       <c r="B362" t="s">
-        <v>857</v>
+        <v>1375</v>
       </c>
       <c r="C362" t="s">
-        <v>858</v>
+        <v>1376</v>
       </c>
       <c r="G362">
         <v>1</v>
@@ -12592,13 +12595,13 @@
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>859</v>
+        <v>386</v>
       </c>
       <c r="B363" t="s">
-        <v>1584</v>
+        <v>857</v>
       </c>
       <c r="C363" t="s">
-        <v>1738</v>
+        <v>858</v>
       </c>
       <c r="G363">
         <v>1</v>
@@ -12606,13 +12609,13 @@
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>387</v>
+        <v>859</v>
       </c>
       <c r="B364" t="s">
-        <v>388</v>
+        <v>1584</v>
       </c>
       <c r="C364" t="s">
-        <v>860</v>
+        <v>1738</v>
       </c>
       <c r="G364">
         <v>1</v>
@@ -12620,13 +12623,13 @@
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>1181</v>
+        <v>387</v>
       </c>
       <c r="B365" t="s">
-        <v>1585</v>
+        <v>388</v>
       </c>
       <c r="C365" t="s">
-        <v>1182</v>
+        <v>860</v>
       </c>
       <c r="G365">
         <v>1</v>
@@ -12634,13 +12637,13 @@
     </row>
     <row r="366" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>389</v>
+        <v>1181</v>
       </c>
       <c r="B366" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C366" t="s">
-        <v>861</v>
+        <v>1182</v>
       </c>
       <c r="G366">
         <v>1</v>
@@ -12648,13 +12651,13 @@
     </row>
     <row r="367" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B367" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="C367" t="s">
-        <v>1740</v>
+        <v>861</v>
       </c>
       <c r="G367">
         <v>1</v>
@@ -12662,13 +12665,13 @@
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B368" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C368" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="G368">
         <v>1</v>
@@ -12676,13 +12679,13 @@
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B369" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C369" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="G369">
         <v>1</v>
@@ -12690,13 +12693,13 @@
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B370" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="C370" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="G370">
         <v>1</v>
@@ -12704,13 +12707,13 @@
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>862</v>
+        <v>393</v>
       </c>
       <c r="B371" t="s">
-        <v>1588</v>
+        <v>1593</v>
       </c>
       <c r="C371" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="G371">
         <v>1</v>
@@ -12718,13 +12721,13 @@
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B372" t="s">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="C372" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="G372">
         <v>1</v>
@@ -12732,13 +12735,13 @@
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B373" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="C373" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="G373">
         <v>1</v>
@@ -12746,13 +12749,13 @@
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>394</v>
+        <v>864</v>
       </c>
       <c r="B374" t="s">
-        <v>865</v>
+        <v>1589</v>
       </c>
       <c r="C374" t="s">
-        <v>866</v>
+        <v>1746</v>
       </c>
       <c r="G374">
         <v>1</v>
@@ -12760,27 +12763,27 @@
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B375" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C375" t="s">
-        <v>868</v>
-      </c>
-      <c r="D375">
+        <v>866</v>
+      </c>
+      <c r="G375">
         <v>1</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B376" t="s">
-        <v>397</v>
+        <v>867</v>
       </c>
       <c r="C376" t="s">
-        <v>398</v>
+        <v>868</v>
       </c>
       <c r="D376">
         <v>1</v>
@@ -12788,41 +12791,41 @@
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B377" t="s">
-        <v>1594</v>
+        <v>397</v>
       </c>
       <c r="C377" t="s">
-        <v>1747</v>
-      </c>
-      <c r="E377">
+        <v>398</v>
+      </c>
+      <c r="D377">
         <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B378" t="s">
-        <v>869</v>
+        <v>1594</v>
       </c>
       <c r="C378" t="s">
-        <v>870</v>
-      </c>
-      <c r="G378">
+        <v>1747</v>
+      </c>
+      <c r="E378">
         <v>1</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>871</v>
+        <v>400</v>
       </c>
       <c r="B379" t="s">
-        <v>1595</v>
+        <v>869</v>
       </c>
       <c r="C379" t="s">
-        <v>1748</v>
+        <v>870</v>
       </c>
       <c r="G379">
         <v>1</v>
@@ -12830,13 +12833,13 @@
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>401</v>
+        <v>871</v>
       </c>
       <c r="B380" t="s">
-        <v>402</v>
+        <v>1595</v>
       </c>
       <c r="C380" t="s">
-        <v>872</v>
+        <v>1748</v>
       </c>
       <c r="G380">
         <v>1</v>
@@ -12844,13 +12847,13 @@
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B381" t="s">
-        <v>873</v>
+        <v>402</v>
       </c>
       <c r="C381" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="G381">
         <v>1</v>
@@ -12858,13 +12861,13 @@
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>875</v>
+        <v>403</v>
       </c>
       <c r="B382" t="s">
-        <v>1596</v>
+        <v>873</v>
       </c>
       <c r="C382" t="s">
-        <v>1739</v>
+        <v>874</v>
       </c>
       <c r="G382">
         <v>1</v>
@@ -12872,13 +12875,13 @@
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>404</v>
+        <v>875</v>
       </c>
       <c r="B383" t="s">
-        <v>405</v>
+        <v>1596</v>
       </c>
       <c r="C383" t="s">
-        <v>876</v>
+        <v>1739</v>
       </c>
       <c r="G383">
         <v>1</v>
@@ -12886,13 +12889,13 @@
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B384" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C384" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="G384">
         <v>1</v>
@@ -12900,13 +12903,13 @@
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B385" t="s">
-        <v>1597</v>
+        <v>407</v>
       </c>
       <c r="C385" t="s">
-        <v>1749</v>
+        <v>877</v>
       </c>
       <c r="G385">
         <v>1</v>
@@ -12914,13 +12917,13 @@
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B386" t="s">
-        <v>410</v>
+        <v>1597</v>
       </c>
       <c r="C386" t="s">
-        <v>411</v>
+        <v>1749</v>
       </c>
       <c r="G386">
         <v>1</v>
@@ -12928,13 +12931,13 @@
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B387" t="s">
-        <v>1598</v>
+        <v>410</v>
       </c>
       <c r="C387" t="s">
-        <v>1750</v>
+        <v>411</v>
       </c>
       <c r="G387">
         <v>1</v>
@@ -12942,7 +12945,7 @@
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>1678</v>
+        <v>412</v>
       </c>
       <c r="B388" t="s">
         <v>1598</v>
@@ -12956,13 +12959,13 @@
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>413</v>
+        <v>1678</v>
       </c>
       <c r="B389" t="s">
-        <v>414</v>
+        <v>1598</v>
       </c>
       <c r="C389" t="s">
-        <v>878</v>
+        <v>1750</v>
       </c>
       <c r="G389">
         <v>1</v>
@@ -12970,13 +12973,13 @@
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>879</v>
+        <v>413</v>
       </c>
       <c r="B390" t="s">
-        <v>1599</v>
+        <v>414</v>
       </c>
       <c r="C390" t="s">
-        <v>1751</v>
+        <v>878</v>
       </c>
       <c r="G390">
         <v>1</v>
@@ -12984,13 +12987,13 @@
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>415</v>
+        <v>879</v>
       </c>
       <c r="B391" t="s">
-        <v>416</v>
+        <v>1599</v>
       </c>
       <c r="C391" t="s">
-        <v>417</v>
+        <v>1751</v>
       </c>
       <c r="G391">
         <v>1</v>
@@ -12998,13 +13001,13 @@
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B392" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C392" t="s">
-        <v>880</v>
+        <v>417</v>
       </c>
       <c r="G392">
         <v>1</v>
@@ -13012,13 +13015,13 @@
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B393" t="s">
         <v>420</v>
       </c>
       <c r="C393" t="s">
-        <v>421</v>
+        <v>880</v>
       </c>
       <c r="G393">
         <v>1</v>
@@ -13026,13 +13029,13 @@
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B394" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C394" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G394">
         <v>1</v>
@@ -13040,13 +13043,13 @@
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B395" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C395" t="s">
-        <v>881</v>
+        <v>424</v>
       </c>
       <c r="G395">
         <v>1</v>
@@ -13054,13 +13057,13 @@
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B396" t="s">
-        <v>1039</v>
+        <v>426</v>
       </c>
       <c r="C396" t="s">
-        <v>1752</v>
+        <v>881</v>
       </c>
       <c r="G396">
         <v>1</v>
@@ -13068,13 +13071,13 @@
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>1679</v>
+        <v>427</v>
       </c>
       <c r="B397" t="s">
-        <v>1680</v>
+        <v>1039</v>
       </c>
       <c r="C397" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="G397">
         <v>1</v>
@@ -13082,10 +13085,10 @@
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="B398" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="C398" t="s">
         <v>1753</v>
@@ -13096,13 +13099,13 @@
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B399" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="C399" t="s">
-        <v>428</v>
+        <v>1753</v>
       </c>
       <c r="G399">
         <v>1</v>
@@ -13110,13 +13113,13 @@
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>429</v>
+        <v>1682</v>
       </c>
       <c r="B400" t="s">
-        <v>882</v>
+        <v>1684</v>
       </c>
       <c r="C400" t="s">
-        <v>883</v>
+        <v>428</v>
       </c>
       <c r="G400">
         <v>1</v>
@@ -13124,13 +13127,13 @@
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B401" t="s">
-        <v>431</v>
+        <v>882</v>
       </c>
       <c r="C401" t="s">
-        <v>432</v>
+        <v>883</v>
       </c>
       <c r="G401">
         <v>1</v>
@@ -13138,13 +13141,13 @@
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>1279</v>
+        <v>430</v>
       </c>
       <c r="B402" t="s">
-        <v>1600</v>
+        <v>431</v>
       </c>
       <c r="C402" t="s">
-        <v>1280</v>
+        <v>432</v>
       </c>
       <c r="G402">
         <v>1</v>
@@ -13152,27 +13155,27 @@
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>1082</v>
+        <v>1279</v>
       </c>
       <c r="B403" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C403" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E403">
+        <v>1280</v>
+      </c>
+      <c r="G403">
         <v>1</v>
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="B404" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C404" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="E404">
         <v>1</v>
@@ -13180,13 +13183,13 @@
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>1045</v>
+        <v>1084</v>
       </c>
       <c r="B405" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C405" t="s">
-        <v>1046</v>
+        <v>1085</v>
       </c>
       <c r="E405">
         <v>1</v>
@@ -13194,91 +13197,91 @@
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>884</v>
+        <v>1045</v>
       </c>
       <c r="B406" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C406" t="s">
-        <v>1754</v>
-      </c>
-      <c r="F406">
+        <v>1046</v>
+      </c>
+      <c r="E406">
         <v>1</v>
       </c>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>433</v>
+        <v>884</v>
       </c>
       <c r="B407" t="s">
-        <v>1605</v>
+        <v>1604</v>
+      </c>
+      <c r="C407" t="s">
+        <v>1754</v>
+      </c>
+      <c r="F407">
+        <v>1</v>
       </c>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B408" t="s">
-        <v>435</v>
-      </c>
-      <c r="C408" t="s">
-        <v>436</v>
-      </c>
-      <c r="G408">
-        <v>1</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>885</v>
+        <v>434</v>
       </c>
       <c r="B409" t="s">
-        <v>1040</v>
+        <v>435</v>
       </c>
       <c r="C409" t="s">
-        <v>1041</v>
-      </c>
-      <c r="D409">
+        <v>436</v>
+      </c>
+      <c r="G409">
         <v>1</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>1086</v>
+        <v>885</v>
       </c>
       <c r="B410" t="s">
-        <v>1606</v>
+        <v>1040</v>
       </c>
       <c r="C410" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E410">
+        <v>1041</v>
+      </c>
+      <c r="D410">
         <v>1</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B411" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C411" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D411">
+        <v>1087</v>
+      </c>
+      <c r="E411">
         <v>1</v>
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>437</v>
+        <v>1088</v>
       </c>
       <c r="B412" t="s">
-        <v>438</v>
+        <v>1607</v>
       </c>
       <c r="C412" t="s">
-        <v>439</v>
+        <v>1089</v>
       </c>
       <c r="D412">
         <v>1</v>
@@ -13286,13 +13289,13 @@
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>886</v>
+        <v>437</v>
       </c>
       <c r="B413" t="s">
-        <v>1377</v>
+        <v>438</v>
       </c>
       <c r="C413" t="s">
-        <v>1378</v>
+        <v>439</v>
       </c>
       <c r="D413">
         <v>1</v>
@@ -13300,13 +13303,13 @@
     </row>
     <row r="414" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B414" t="s">
-        <v>1608</v>
+        <v>1377</v>
       </c>
       <c r="C414" t="s">
-        <v>955</v>
+        <v>1378</v>
       </c>
       <c r="D414">
         <v>1</v>
@@ -13314,13 +13317,13 @@
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B415" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C415" t="s">
-        <v>1755</v>
+        <v>955</v>
       </c>
       <c r="D415">
         <v>1</v>
@@ -13328,49 +13331,49 @@
     </row>
     <row r="416" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B416" t="s">
-        <v>1610</v>
+        <v>1609</v>
+      </c>
+      <c r="C416" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D416">
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>1135</v>
+        <v>889</v>
       </c>
       <c r="B417" t="s">
-        <v>1611</v>
-      </c>
-      <c r="C417" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E417">
-        <v>1</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>440</v>
+        <v>1135</v>
       </c>
       <c r="B418" t="s">
-        <v>890</v>
+        <v>1611</v>
       </c>
       <c r="C418" t="s">
-        <v>891</v>
-      </c>
-      <c r="D418">
+        <v>1136</v>
+      </c>
+      <c r="E418">
         <v>1</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>892</v>
+        <v>440</v>
       </c>
       <c r="B419" t="s">
-        <v>1612</v>
+        <v>890</v>
       </c>
       <c r="C419" t="s">
-        <v>1756</v>
+        <v>891</v>
       </c>
       <c r="D419">
         <v>1</v>
@@ -13378,27 +13381,27 @@
     </row>
     <row r="420" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>1137</v>
+        <v>892</v>
       </c>
       <c r="B420" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="C420" t="s">
-        <v>1138</v>
-      </c>
-      <c r="H420">
+        <v>1756</v>
+      </c>
+      <c r="D420">
         <v>1</v>
       </c>
     </row>
     <row r="421" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>1221</v>
+        <v>1137</v>
       </c>
       <c r="B421" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="C421" t="s">
-        <v>1222</v>
+        <v>1138</v>
       </c>
       <c r="H421">
         <v>1</v>
@@ -13406,69 +13409,69 @@
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>441</v>
+        <v>1221</v>
       </c>
       <c r="B422" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="C422" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D422">
+        <v>1222</v>
+      </c>
+      <c r="H422">
         <v>1</v>
       </c>
     </row>
     <row r="423" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>893</v>
+        <v>441</v>
       </c>
       <c r="B423" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C423" t="s">
-        <v>1758</v>
-      </c>
-      <c r="F423">
+        <v>1757</v>
+      </c>
+      <c r="D423">
         <v>1</v>
       </c>
     </row>
     <row r="424" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>1281</v>
+        <v>893</v>
       </c>
       <c r="B424" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C424" t="s">
-        <v>1282</v>
-      </c>
-      <c r="D424">
+        <v>1758</v>
+      </c>
+      <c r="F424">
         <v>1</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>894</v>
+        <v>1281</v>
       </c>
       <c r="B425" t="s">
-        <v>895</v>
+        <v>1617</v>
       </c>
       <c r="C425" t="s">
-        <v>896</v>
-      </c>
-      <c r="F425">
+        <v>1282</v>
+      </c>
+      <c r="D425">
         <v>1</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B426" t="s">
-        <v>1618</v>
+        <v>895</v>
       </c>
       <c r="C426" t="s">
-        <v>1759</v>
+        <v>896</v>
       </c>
       <c r="F426">
         <v>1</v>
@@ -13476,10 +13479,10 @@
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B427" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C427" t="s">
         <v>1759</v>
@@ -13490,77 +13493,77 @@
     </row>
     <row r="428" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>1197</v>
+        <v>898</v>
       </c>
       <c r="B428" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C428" t="s">
-        <v>1198</v>
-      </c>
-      <c r="H428">
+        <v>1759</v>
+      </c>
+      <c r="F428">
         <v>1</v>
       </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>442</v>
+        <v>1197</v>
       </c>
       <c r="B429" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C429" t="s">
-        <v>1760</v>
-      </c>
-      <c r="E429">
+        <v>1198</v>
+      </c>
+      <c r="H429">
         <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="B430" t="s">
-        <v>1036</v>
+        <v>1621</v>
       </c>
       <c r="C430" t="s">
-        <v>1037</v>
+        <v>1760</v>
+      </c>
+      <c r="E430">
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>899</v>
+        <v>466</v>
       </c>
       <c r="B431" t="s">
-        <v>1002</v>
+        <v>1036</v>
       </c>
       <c r="C431" t="s">
-        <v>1622</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B432" t="s">
-        <v>1623</v>
+        <v>1002</v>
       </c>
       <c r="C432" t="s">
-        <v>1761</v>
-      </c>
-      <c r="F432">
-        <v>1</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>1139</v>
+        <v>900</v>
       </c>
       <c r="B433" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C433" t="s">
-        <v>1140</v>
+        <v>1761</v>
       </c>
       <c r="F433">
         <v>1</v>
@@ -13568,13 +13571,13 @@
     </row>
     <row r="434" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>901</v>
+        <v>1139</v>
       </c>
       <c r="B434" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C434" t="s">
-        <v>1761</v>
+        <v>1140</v>
       </c>
       <c r="F434">
         <v>1</v>
@@ -13582,13 +13585,13 @@
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>1141</v>
+        <v>901</v>
       </c>
       <c r="B435" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C435" t="s">
-        <v>1142</v>
+        <v>1761</v>
       </c>
       <c r="F435">
         <v>1</v>
@@ -13596,13 +13599,13 @@
     </row>
     <row r="436" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>1055</v>
+        <v>1141</v>
       </c>
       <c r="B436" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C436" t="s">
-        <v>1056</v>
+        <v>1142</v>
       </c>
       <c r="F436">
         <v>1</v>
@@ -13610,41 +13613,41 @@
     </row>
     <row r="437" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>443</v>
+        <v>1055</v>
       </c>
       <c r="B437" t="s">
-        <v>444</v>
+        <v>1627</v>
       </c>
       <c r="C437" t="s">
-        <v>445</v>
-      </c>
-      <c r="D437">
+        <v>1056</v>
+      </c>
+      <c r="F437">
         <v>1</v>
       </c>
     </row>
     <row r="438" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>1143</v>
+        <v>443</v>
       </c>
       <c r="B438" t="s">
-        <v>1628</v>
+        <v>444</v>
       </c>
       <c r="C438" t="s">
-        <v>1044</v>
-      </c>
-      <c r="F438">
+        <v>445</v>
+      </c>
+      <c r="D438">
         <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B439" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C439" t="s">
-        <v>1145</v>
+        <v>1044</v>
       </c>
       <c r="F439">
         <v>1</v>
@@ -13652,13 +13655,13 @@
     </row>
     <row r="440" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>1199</v>
+        <v>1144</v>
       </c>
       <c r="B440" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C440" t="s">
-        <v>1200</v>
+        <v>1145</v>
       </c>
       <c r="F440">
         <v>1</v>
@@ -13666,13 +13669,13 @@
     </row>
     <row r="441" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="B441" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C441" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="F441">
         <v>1</v>
@@ -13680,13 +13683,13 @@
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B442" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C442" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="F442">
         <v>1</v>
@@ -13694,66 +13697,66 @@
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>1090</v>
+        <v>1203</v>
       </c>
       <c r="B443" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C443" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E443">
+        <v>1204</v>
+      </c>
+      <c r="F443">
         <v>1</v>
       </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>902</v>
+        <v>1090</v>
       </c>
       <c r="B444" t="s">
-        <v>1038</v>
+        <v>1633</v>
       </c>
       <c r="C444" t="s">
-        <v>1762</v>
-      </c>
-      <c r="H444">
+        <v>1091</v>
+      </c>
+      <c r="E444">
         <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B445" t="s">
-        <v>1634</v>
-      </c>
-      <c r="G445">
+        <v>1038</v>
+      </c>
+      <c r="C445" t="s">
+        <v>1762</v>
+      </c>
+      <c r="H445">
         <v>1</v>
       </c>
     </row>
     <row r="446" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>1146</v>
+        <v>903</v>
       </c>
       <c r="B446" t="s">
-        <v>1635</v>
-      </c>
-      <c r="C446" t="s">
-        <v>1147</v>
-      </c>
-      <c r="H446">
+        <v>1634</v>
+      </c>
+      <c r="G446">
         <v>1</v>
       </c>
     </row>
     <row r="447" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="B447" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C447" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="H447">
         <v>1</v>
@@ -13761,13 +13764,13 @@
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="B448" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C448" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="H448">
         <v>1</v>
@@ -13775,13 +13778,13 @@
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B449" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C449" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="H449">
         <v>1</v>
@@ -13789,27 +13792,27 @@
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>904</v>
+        <v>1152</v>
       </c>
       <c r="B450" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C450" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F450">
+        <v>1153</v>
+      </c>
+      <c r="H450">
         <v>1</v>
       </c>
     </row>
     <row r="451" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>1057</v>
+        <v>904</v>
       </c>
       <c r="B451" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C451" t="s">
-        <v>1058</v>
+        <v>1763</v>
       </c>
       <c r="F451">
         <v>1</v>
@@ -13817,13 +13820,13 @@
     </row>
     <row r="452" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B452" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C452" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="F452">
         <v>1</v>
@@ -13831,13 +13834,13 @@
     </row>
     <row r="453" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>1205</v>
+        <v>1059</v>
       </c>
       <c r="B453" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="C453" t="s">
-        <v>1206</v>
+        <v>1060</v>
       </c>
       <c r="F453">
         <v>1</v>
@@ -13845,13 +13848,13 @@
     </row>
     <row r="454" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>446</v>
+        <v>1205</v>
       </c>
       <c r="B454" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="C454" t="s">
-        <v>905</v>
+        <v>1206</v>
       </c>
       <c r="F454">
         <v>1</v>
@@ -13859,13 +13862,13 @@
     </row>
     <row r="455" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>1154</v>
+        <v>446</v>
       </c>
       <c r="B455" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="C455" t="s">
-        <v>1155</v>
+        <v>905</v>
       </c>
       <c r="F455">
         <v>1</v>
@@ -13873,27 +13876,27 @@
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>1183</v>
+        <v>1154</v>
       </c>
       <c r="B456" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="C456" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G456">
+        <v>1155</v>
+      </c>
+      <c r="F456">
         <v>1</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>906</v>
+        <v>1183</v>
       </c>
       <c r="B457" t="s">
-        <v>907</v>
+        <v>1646</v>
       </c>
       <c r="C457" t="s">
-        <v>908</v>
+        <v>1184</v>
       </c>
       <c r="G457">
         <v>1</v>
@@ -13901,13 +13904,13 @@
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="B458" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="C458" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="G458">
         <v>1</v>
@@ -13915,13 +13918,13 @@
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B459" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="C459" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="G459">
         <v>1</v>
@@ -13929,13 +13932,13 @@
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="B460" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C460" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="G460">
         <v>1</v>
@@ -13943,13 +13946,13 @@
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>447</v>
+        <v>915</v>
       </c>
       <c r="B461" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="C461" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="G461">
         <v>1</v>
@@ -13957,10 +13960,13 @@
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>918</v>
+        <v>447</v>
       </c>
       <c r="B462" t="s">
-        <v>919</v>
+        <v>920</v>
+      </c>
+      <c r="C462" t="s">
+        <v>921</v>
       </c>
       <c r="G462">
         <v>1</v>
@@ -13968,13 +13974,10 @@
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="B463" t="s">
-        <v>923</v>
-      </c>
-      <c r="C463" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="G463">
         <v>1</v>
@@ -13982,13 +13985,13 @@
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>1185</v>
+        <v>922</v>
       </c>
       <c r="B464" t="s">
-        <v>1645</v>
+        <v>923</v>
       </c>
       <c r="C464" t="s">
-        <v>1186</v>
+        <v>924</v>
       </c>
       <c r="G464">
         <v>1</v>
@@ -13996,13 +13999,13 @@
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>925</v>
+        <v>1185</v>
       </c>
       <c r="B465" t="s">
-        <v>926</v>
+        <v>1645</v>
       </c>
       <c r="C465" t="s">
-        <v>926</v>
+        <v>1186</v>
       </c>
       <c r="G465">
         <v>1</v>
@@ -14010,13 +14013,13 @@
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B466" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C466" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G466">
         <v>1</v>
@@ -14024,13 +14027,13 @@
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="B467" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C467" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G467">
         <v>1</v>
@@ -14038,13 +14041,13 @@
     </row>
     <row r="468" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B468" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C468" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G468">
         <v>1</v>
@@ -14052,13 +14055,13 @@
     </row>
     <row r="469" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B469" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C469" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="G469">
         <v>1</v>
@@ -14066,13 +14069,13 @@
     </row>
     <row r="470" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B470" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C470" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="G470">
         <v>1</v>
@@ -14080,13 +14083,13 @@
     </row>
     <row r="471" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B471" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C471" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="G471">
         <v>1</v>
@@ -14094,13 +14097,13 @@
     </row>
     <row r="472" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B472" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C472" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="G472">
         <v>1</v>
@@ -14108,13 +14111,13 @@
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B473" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C473" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G473">
         <v>1</v>
@@ -14122,13 +14125,13 @@
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B474" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C474" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G474">
         <v>1</v>
@@ -14136,27 +14139,27 @@
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B475" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C475" t="s">
-        <v>946</v>
-      </c>
-      <c r="H475">
+        <v>944</v>
+      </c>
+      <c r="G475">
         <v>1</v>
       </c>
     </row>
     <row r="476" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B476" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C476" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="H476">
         <v>1</v>
@@ -14164,13 +14167,13 @@
     </row>
     <row r="477" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>448</v>
+        <v>947</v>
       </c>
       <c r="B477" t="s">
-        <v>449</v>
+        <v>948</v>
       </c>
       <c r="C477" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H477">
         <v>1</v>
@@ -14178,13 +14181,13 @@
     </row>
     <row r="478" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>950</v>
+        <v>448</v>
       </c>
       <c r="B478" t="s">
-        <v>951</v>
+        <v>449</v>
       </c>
       <c r="C478" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="H478">
         <v>1</v>
@@ -14192,10 +14195,13 @@
     </row>
     <row r="479" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>464</v>
+        <v>950</v>
       </c>
       <c r="B479" t="s">
-        <v>465</v>
+        <v>951</v>
+      </c>
+      <c r="C479" t="s">
+        <v>952</v>
       </c>
       <c r="H479">
         <v>1</v>
@@ -14203,41 +14209,38 @@
     </row>
     <row r="480" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="B480" t="s">
-        <v>451</v>
-      </c>
-      <c r="C480" t="s">
-        <v>452</v>
-      </c>
-      <c r="G480">
+        <v>465</v>
+      </c>
+      <c r="H480">
         <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>1156</v>
+        <v>450</v>
       </c>
       <c r="B481" t="s">
-        <v>1647</v>
+        <v>451</v>
       </c>
       <c r="C481" t="s">
-        <v>1157</v>
-      </c>
-      <c r="H481">
+        <v>452</v>
+      </c>
+      <c r="G481">
         <v>1</v>
       </c>
     </row>
     <row r="482" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="B482" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="C482" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="H482">
         <v>1</v>
@@ -14245,13 +14248,13 @@
     </row>
     <row r="483" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>453</v>
+        <v>1158</v>
       </c>
       <c r="B483" t="s">
-        <v>454</v>
+        <v>1648</v>
       </c>
       <c r="C483" t="s">
-        <v>455</v>
+        <v>1159</v>
       </c>
       <c r="H483">
         <v>1</v>
@@ -14259,13 +14262,13 @@
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>1160</v>
+        <v>453</v>
       </c>
       <c r="B484" t="s">
-        <v>1649</v>
+        <v>454</v>
       </c>
       <c r="C484" t="s">
-        <v>1128</v>
+        <v>455</v>
       </c>
       <c r="H484">
         <v>1</v>
@@ -14273,13 +14276,13 @@
     </row>
     <row r="485" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B485" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="C485" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="H485">
         <v>1</v>
@@ -14287,13 +14290,13 @@
     </row>
     <row r="486" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>1067</v>
+        <v>1161</v>
       </c>
       <c r="B486" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C486" t="s">
-        <v>1054</v>
+        <v>1130</v>
       </c>
       <c r="H486">
         <v>1</v>
@@ -14301,13 +14304,13 @@
     </row>
     <row r="487" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>456</v>
+        <v>1067</v>
       </c>
       <c r="B487" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="C487" t="s">
-        <v>953</v>
+        <v>1054</v>
       </c>
       <c r="H487">
         <v>1</v>
@@ -14315,13 +14318,13 @@
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B488" t="s">
-        <v>458</v>
+        <v>1652</v>
       </c>
       <c r="C488" t="s">
-        <v>459</v>
+        <v>953</v>
       </c>
       <c r="H488">
         <v>1</v>
@@ -14329,27 +14332,27 @@
     </row>
     <row r="489" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B489" t="s">
-        <v>954</v>
+        <v>458</v>
       </c>
       <c r="C489" t="s">
-        <v>955</v>
-      </c>
-      <c r="D489">
+        <v>459</v>
+      </c>
+      <c r="H489">
         <v>1</v>
       </c>
     </row>
     <row r="490" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B490" t="s">
-        <v>462</v>
+        <v>954</v>
       </c>
       <c r="C490" t="s">
-        <v>463</v>
+        <v>955</v>
       </c>
       <c r="D490">
         <v>1</v>
@@ -14357,49 +14360,49 @@
     </row>
     <row r="491" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>1697</v>
+        <v>461</v>
       </c>
       <c r="B491" t="s">
-        <v>1698</v>
-      </c>
-      <c r="G491">
+        <v>462</v>
+      </c>
+      <c r="C491" t="s">
+        <v>463</v>
+      </c>
+      <c r="D491">
         <v>1</v>
       </c>
     </row>
     <row r="492" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>1702</v>
+        <v>1697</v>
       </c>
       <c r="B492" t="s">
-        <v>1703</v>
-      </c>
-      <c r="F492">
+        <v>1698</v>
+      </c>
+      <c r="G492">
         <v>1</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="B493" t="s">
-        <v>1575</v>
-      </c>
-      <c r="C493" t="s">
-        <v>1764</v>
-      </c>
-      <c r="G493">
+        <v>1703</v>
+      </c>
+      <c r="F493">
         <v>1</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B494" t="s">
-        <v>1706</v>
+        <v>1575</v>
       </c>
       <c r="C494" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="G494">
         <v>1</v>
@@ -14407,13 +14410,13 @@
     </row>
     <row r="495" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="B495" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="C495" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="G495">
         <v>1</v>
@@ -14421,38 +14424,38 @@
     </row>
     <row r="496" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="B496" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="C496" t="s">
-        <v>1767</v>
-      </c>
-      <c r="D496">
+        <v>1766</v>
+      </c>
+      <c r="G496">
         <v>1</v>
       </c>
     </row>
     <row r="497" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="B497" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="C497" t="s">
-        <v>1750</v>
-      </c>
-      <c r="H497">
+        <v>1767</v>
+      </c>
+      <c r="D497">
         <v>1</v>
       </c>
     </row>
     <row r="498" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>1700</v>
+        <v>1711</v>
       </c>
       <c r="B498" t="s">
-        <v>1701</v>
+        <v>1712</v>
       </c>
       <c r="C498" t="s">
         <v>1750</v>
@@ -14463,10 +14466,10 @@
     </row>
     <row r="499" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>1713</v>
+        <v>1700</v>
       </c>
       <c r="B499" t="s">
-        <v>414</v>
+        <v>1701</v>
       </c>
       <c r="C499" t="s">
         <v>1750</v>
@@ -14477,34 +14480,48 @@
     </row>
     <row r="500" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B500" t="s">
-        <v>1715</v>
+        <v>414</v>
       </c>
       <c r="C500" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G500">
+        <v>1750</v>
+      </c>
+      <c r="H500">
         <v>1</v>
       </c>
     </row>
     <row r="501" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A502" t="s">
         <v>1699</v>
       </c>
-      <c r="B501" t="s">
+      <c r="B502" t="s">
         <v>1716</v>
       </c>
-      <c r="C501" t="s">
+      <c r="C502" t="s">
         <v>459</v>
       </c>
-      <c r="H501">
+      <c r="H502">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I501" xr:uid="{00000000-0001-0000-0B00-000000000000}"/>
+  <autoFilter ref="A1:I502" xr:uid="{00000000-0001-0000-0B00-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>